<commit_message>
2022Q2 DCF Update for LiquidityServices (LQDT)
Pretty fairly valued.
Price target: $16.63
</commit_message>
<xml_diff>
--- a/DCF Models/LQDT.xlsx
+++ b/DCF Models/LQDT.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Desktop\Fiduciary\investingModels\Models\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Desktop\Fiduciary\investingModels\DCF Models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D83485DA-1E0A-49C6-810F-DBF85795A534}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6916840-01D2-4066-A710-004091EDCAC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20565" yWindow="6090" windowWidth="24360" windowHeight="13650" xr2:uid="{F1620845-D3A1-42C3-B09D-9C0C2CC1B833}"/>
+    <workbookView xWindow="1335" yWindow="390" windowWidth="34665" windowHeight="13410" activeTab="1" xr2:uid="{F1620845-D3A1-42C3-B09D-9C0C2CC1B833}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="2" r:id="rId1"/>
@@ -20,14 +20,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -749,8 +741,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AABCF078-8F80-46BC-B5B9-A1A85F980B56}">
   <dimension ref="B1:O19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O24" sqref="O24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -883,11 +875,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5852247D-41DC-4DAB-8C48-410CF359BD4C}">
   <dimension ref="A1:DE59"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C38" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="O23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="N23" sqref="N23"/>
+      <selection pane="bottomRight" activeCell="AL42" sqref="AL42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>